<commit_message>
fix: Update HMI_COMMAND Excel file to reflect latest changes
</commit_message>
<xml_diff>
--- a/S7-1200-1500/Core/HMI/__HMI_COMMAND__-v1.0.xlsx
+++ b/S7-1200-1500/Core/HMI/__HMI_COMMAND__-v1.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.2\work\A06_TO\03_PLC\90_Library\HMI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.0.2\work\PlcFramework\S7-1200-1500\Core\HMI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2125F3E5-1D36-4866-A004-92B3C23EF9D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939CC84E-6245-4DF6-B9E8-28ED671D79FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19455" yWindow="16200" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="450" yWindow="1455" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Constants" sheetId="2" r:id="rId1"/>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{444032EF-0904-40D8-BE6E-8501789D19DC}">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="E58" sqref="E58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>